<commit_message>
autosum and average option in excel
</commit_message>
<xml_diff>
--- a/ExcelEssesntialTraining-Office365/Ch-03-Formulas.xlsx
+++ b/ExcelEssesntialTraining-Office365/Ch-03-Formulas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/satya/Data/General-Learning/LearnExcel/ExcelEssesntialTraining-Office365/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D81B59B9-FEAF-9041-8B85-93E851B38796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C55EBC3-40DC-AA47-8561-28A035E7B6BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4700" yWindow="3200" windowWidth="27240" windowHeight="16440" activeTab="3" xr2:uid="{971B0534-D4EF-5445-8182-3FDEEF3B6ED9}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Formulas" sheetId="3" r:id="rId3"/>
     <sheet name="SumAverage" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
   <si>
     <t>Sales</t>
   </si>
@@ -235,6 +235,27 @@
   </si>
   <si>
     <t>Latin America</t>
+  </si>
+  <si>
+    <t>Click autosum option under home tab ribbon options</t>
+  </si>
+  <si>
+    <t>Select all columns plus empty columns where sum should happne and click autosum option under home tab ribbon options</t>
+  </si>
+  <si>
+    <t>Orange is for all columns should be used for sum</t>
+  </si>
+  <si>
+    <t>Yellow is the empty columns where sum must be computed before autosum option</t>
+  </si>
+  <si>
+    <t>Yellow is the empty columns where average must be computed before average option</t>
+  </si>
+  <si>
+    <t>Orange is for all columns should be used for average</t>
+  </si>
+  <si>
+    <t>Select all columns plus empty columns where average should happne and click average option under home tab ribbon options</t>
   </si>
 </sst>
 </file>
@@ -242,7 +263,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -286,7 +307,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -305,6 +326,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -318,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -332,7 +365,11 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1148,15 +1185,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74799B9D-CC99-1D44-B555-D6D4208E89EB}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="7"/>
       <c r="B1" s="8" t="s">
         <v>51</v>
@@ -1178,7 +1215,7 @@
       </c>
       <c r="H1" s="9"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>57</v>
       </c>
@@ -1197,10 +1234,16 @@
       <c r="F2" s="7">
         <v>154</v>
       </c>
-      <c r="G2" s="7"/>
+      <c r="G2" s="7">
+        <f>SUM(B2:F2)</f>
+        <v>576</v>
+      </c>
       <c r="H2" s="9"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="10"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -1210,7 +1253,7 @@
       <c r="G3" s="7"/>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="11"/>
       <c r="C4" s="7"/>
@@ -1220,7 +1263,7 @@
       <c r="G4" s="7"/>
       <c r="H4" s="9"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>58</v>
       </c>
@@ -1236,7 +1279,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>59</v>
       </c>
@@ -1252,7 +1295,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>60</v>
       </c>
@@ -1272,7 +1315,7 @@
       </c>
       <c r="H7" s="9"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>61</v>
       </c>
@@ -1286,17 +1329,22 @@
       <c r="G8" s="7"/>
       <c r="H8" s="9"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
+      <c r="B9" s="11">
+        <f>SUM(B5:B8)</f>
+        <v>25096</v>
+      </c>
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="9"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="B10" s="11"/>
       <c r="C10" s="7"/>
@@ -1306,7 +1354,7 @@
       <c r="G10" s="7"/>
       <c r="H10" s="9"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="8" t="s">
         <v>3</v>
@@ -1328,101 +1376,318 @@
       </c>
       <c r="H11" s="9"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="12">
         <v>13</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="12">
         <v>21</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="12">
         <v>13</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="12">
         <v>17</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="12">
         <v>18</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="12">
         <v>25</v>
       </c>
-      <c r="H12" s="9"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H12" s="14">
+        <f>SUM(B12:G12)</f>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="12">
         <v>11</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="12">
         <v>12</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="12">
         <v>10</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="12">
         <v>15</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="12">
         <v>14</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="12">
         <v>17</v>
       </c>
-      <c r="H13" s="9"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H13" s="14">
+        <f>SUM(B13:G13)</f>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="12">
         <v>14</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="12">
         <v>17</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="12">
         <v>16</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="12">
         <v>13</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="12">
         <v>15</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="12">
         <v>19</v>
       </c>
-      <c r="H14" s="9"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H14" s="14">
+        <f>SUM(B14:G14)</f>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="12">
         <v>5</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="12">
         <v>11</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="12">
         <v>7</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="12">
         <v>11</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="12">
         <v>9</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="12">
         <v>13</v>
       </c>
-      <c r="H15" s="9"/>
+      <c r="H15" s="14">
+        <f>SUM(B15:G15)</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="13">
+        <f>SUM(B12:B15)</f>
+        <v>43</v>
+      </c>
+      <c r="C16" s="13">
+        <f>SUM(C12:C15)</f>
+        <v>61</v>
+      </c>
+      <c r="D16" s="13">
+        <f>SUM(D12:D15)</f>
+        <v>46</v>
+      </c>
+      <c r="E16" s="13">
+        <f>SUM(E12:E15)</f>
+        <v>56</v>
+      </c>
+      <c r="F16" s="13">
+        <f>SUM(F12:F15)</f>
+        <v>56</v>
+      </c>
+      <c r="G16" s="13">
+        <f>SUM(G12:G15)</f>
+        <v>74</v>
+      </c>
+      <c r="H16" s="14">
+        <f>SUM(H12:H15)</f>
+        <v>336</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="7"/>
+      <c r="B23" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="9"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="12">
+        <v>13</v>
+      </c>
+      <c r="C24" s="12">
+        <v>21</v>
+      </c>
+      <c r="D24" s="12">
+        <v>13</v>
+      </c>
+      <c r="E24" s="12">
+        <v>17</v>
+      </c>
+      <c r="F24" s="12">
+        <v>18</v>
+      </c>
+      <c r="G24" s="12">
+        <v>25</v>
+      </c>
+      <c r="H24" s="15"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="12">
+        <v>11</v>
+      </c>
+      <c r="C25" s="12">
+        <v>12</v>
+      </c>
+      <c r="D25" s="12">
+        <v>10</v>
+      </c>
+      <c r="E25" s="12">
+        <v>15</v>
+      </c>
+      <c r="F25" s="12">
+        <v>14</v>
+      </c>
+      <c r="G25" s="12">
+        <v>17</v>
+      </c>
+      <c r="H25" s="15"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="12">
+        <v>14</v>
+      </c>
+      <c r="C26" s="12">
+        <v>17</v>
+      </c>
+      <c r="D26" s="12">
+        <v>16</v>
+      </c>
+      <c r="E26" s="12">
+        <v>13</v>
+      </c>
+      <c r="F26" s="12">
+        <v>15</v>
+      </c>
+      <c r="G26" s="12">
+        <v>19</v>
+      </c>
+      <c r="H26" s="15"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="12">
+        <v>5</v>
+      </c>
+      <c r="C27" s="12">
+        <v>11</v>
+      </c>
+      <c r="D27" s="12">
+        <v>7</v>
+      </c>
+      <c r="E27" s="12">
+        <v>11</v>
+      </c>
+      <c r="F27" s="12">
+        <v>9</v>
+      </c>
+      <c r="G27" s="12">
+        <v>13</v>
+      </c>
+      <c r="H27" s="15"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="13">
+        <f>AVERAGE(B24:B27)</f>
+        <v>10.75</v>
+      </c>
+      <c r="C28" s="13">
+        <f>AVERAGE(C24:C27)</f>
+        <v>15.25</v>
+      </c>
+      <c r="D28" s="13">
+        <f>AVERAGE(D24:D27)</f>
+        <v>11.5</v>
+      </c>
+      <c r="E28" s="13">
+        <f>AVERAGE(E24:E27)</f>
+        <v>14</v>
+      </c>
+      <c r="F28" s="13">
+        <f>AVERAGE(F24:F27)</f>
+        <v>14</v>
+      </c>
+      <c r="G28" s="13">
+        <f>AVERAGE(G24:G27)</f>
+        <v>18.5</v>
+      </c>
+      <c r="H28" s="15"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
best fit size of column
</commit_message>
<xml_diff>
--- a/ExcelEssesntialTraining-Office365/Ch-03-Formulas.xlsx
+++ b/ExcelEssesntialTraining-Office365/Ch-03-Formulas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/satya/Data/General-Learning/LearnExcel/ExcelEssesntialTraining-Office365/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD55B5C9-E9A4-4244-ACF2-FD6610227B4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC296E7-8E79-6C45-832E-49CFE8420BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4700" yWindow="3200" windowWidth="27240" windowHeight="16440" activeTab="5" xr2:uid="{971B0534-D4EF-5445-8182-3FDEEF3B6ED9}"/>
+    <workbookView xWindow="4700" yWindow="3200" windowWidth="27240" windowHeight="16440" activeTab="6" xr2:uid="{971B0534-D4EF-5445-8182-3FDEEF3B6ED9}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Entry" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="SumAverage" sheetId="4" r:id="rId4"/>
     <sheet name="xlookup" sheetId="5" r:id="rId5"/>
     <sheet name="Superscript-Subscript" sheetId="6" r:id="rId6"/>
+    <sheet name="BestFit" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4897" uniqueCount="883">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4903" uniqueCount="889">
   <si>
     <t>Sales</t>
   </si>
@@ -2718,6 +2719,24 @@
       </rPr>
       <t>O</t>
     </r>
+  </si>
+  <si>
+    <t>Hello hi there</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cool </t>
+  </si>
+  <si>
+    <t>are you</t>
+  </si>
+  <si>
+    <t>simple fit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not at all </t>
+  </si>
+  <si>
+    <t>Select upper right corner for complete workshhet and double click when + sign appears</t>
   </si>
 </sst>
 </file>
@@ -2969,7 +2988,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -3075,6 +3094,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="10" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{46CBC3A7-FB58-1D43-9B13-D4752CFDE41C}"/>
@@ -4408,7 +4428,7 @@
   <dimension ref="A1:Z763"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -40555,11 +40575,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A86664-BC4F-7F4C-8FEB-F78C7F497787}">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="85.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -40594,4 +40617,51 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE9CF16F-0C47-754B-B712-21A753C10812}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>883</v>
+      </c>
+      <c r="B1" t="s">
+        <v>884</v>
+      </c>
+      <c r="C1" t="s">
+        <v>885</v>
+      </c>
+      <c r="D1" s="52">
+        <v>123456788900</v>
+      </c>
+      <c r="E1" t="s">
+        <v>886</v>
+      </c>
+      <c r="F1" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>888</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>